<commit_message>
front and top view are accomplished
</commit_message>
<xml_diff>
--- a/initial_data.xlsx
+++ b/initial_data.xlsx
@@ -227,12 +227,39 @@
         </r>
       </text>
     </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t>Пронькин Дмитрий Юрьевич:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">
+Bolt holes diameter
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -313,9 +340,6 @@
   </si>
   <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>Quantity</t>
   </si>
   <si>
     <t>Row indents</t>
@@ -386,8 +410,38 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(CHORDS)</t>
+      <t>(middle)</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Bolt holes on the right edge of the element </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(wall)</t>
+    </r>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>x left</t>
+  </si>
+  <si>
+    <t>x right</t>
+  </si>
+  <si>
+    <t>x middle</t>
   </si>
 </sst>
 </file>
@@ -461,7 +515,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,6 +525,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -838,7 +898,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -862,12 +922,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -958,34 +1012,52 @@
     <xf numFmtId="1" fontId="6" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1292,10 +1364,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:Z44"/>
+  <dimension ref="A1:Z87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O4:O5"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="H76" sqref="H76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,35 +1380,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="13" t="s">
         <v>8</v>
+      </c>
+      <c r="K1" s="47" t="s">
+        <v>42</v>
       </c>
       <c r="Y1" s="4" t="s">
         <v>9</v>
@@ -1346,10 +1421,10 @@
       </c>
     </row>
     <row r="2" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="52" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="49">
@@ -1376,7 +1451,9 @@
       <c r="J2" s="50">
         <v>12</v>
       </c>
-      <c r="K2" s="1"/>
+      <c r="K2" s="50">
+        <v>25</v>
+      </c>
       <c r="Y2" s="6" t="s">
         <v>12</v>
       </c>
@@ -1385,48 +1462,48 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
       <c r="K3" s="1"/>
       <c r="Y3" s="6"/>
       <c r="Z3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
-      <c r="J4" s="17"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
       <c r="K4" s="1"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="43"/>
+      <c r="A5" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="54"/>
+      <c r="C5" s="54"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="54"/>
+      <c r="F5" s="54"/>
+      <c r="G5" s="54"/>
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="46"/>
       <c r="K5" s="1"/>
       <c r="Y5" s="6" t="s">
         <v>13</v>
@@ -1436,82 +1513,76 @@
       </c>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="21">
+        <v>4</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="23">
-        <v>4</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="23"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="27" t="s">
+      <c r="H7" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I7" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="1"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="30">
+      <c r="B8" s="28">
         <v>50</v>
       </c>
-      <c r="C8" s="30">
-        <v>4</v>
-      </c>
-      <c r="D8" s="30">
+      <c r="C8" s="28">
         <v>50</v>
       </c>
-      <c r="E8" s="30">
-        <v>80</v>
-      </c>
-      <c r="F8" s="30">
+      <c r="D8" s="28">
+        <v>80</v>
+      </c>
+      <c r="E8" s="28">
         <v>160</v>
       </c>
-      <c r="G8" s="30">
-        <v>80</v>
-      </c>
-      <c r="H8" s="40"/>
-      <c r="I8" s="40"/>
-      <c r="J8" s="40"/>
+      <c r="F8" s="28">
+        <v>80</v>
+      </c>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="5"/>
       <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
+      <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
       <c r="Q8" s="5"/>
@@ -1523,36 +1594,33 @@
       <c r="W8" s="5"/>
       <c r="X8" s="5"/>
       <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="20">
-        <v>80</v>
-      </c>
-      <c r="C9" s="20">
-        <v>4</v>
-      </c>
-      <c r="D9" s="20">
+      <c r="B9" s="18">
+        <v>80</v>
+      </c>
+      <c r="C9" s="18">
         <v>50</v>
       </c>
-      <c r="E9" s="20">
-        <v>80</v>
-      </c>
-      <c r="F9" s="20">
+      <c r="D9" s="18">
+        <v>80</v>
+      </c>
+      <c r="E9" s="18">
         <v>160</v>
       </c>
-      <c r="G9" s="20">
-        <v>80</v>
-      </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="40"/>
+      <c r="F9" s="18">
+        <v>80</v>
+      </c>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="6"/>
       <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="16"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="6"/>
@@ -1565,133 +1633,124 @@
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="20">
-        <v>80</v>
-      </c>
-      <c r="C10" s="20">
-        <v>2</v>
-      </c>
-      <c r="D10" s="20">
+      <c r="B10" s="18">
+        <v>80</v>
+      </c>
+      <c r="C10" s="18">
         <v>50</v>
       </c>
-      <c r="E10" s="20">
+      <c r="D10" s="18">
         <v>320</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="16"/>
-      <c r="N10" s="6"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="20">
-        <v>80</v>
-      </c>
-      <c r="C11" s="20">
-        <v>2</v>
-      </c>
-      <c r="D11" s="20">
+      <c r="B11" s="18">
+        <v>80</v>
+      </c>
+      <c r="C11" s="18">
         <v>130</v>
       </c>
-      <c r="E11" s="20">
+      <c r="D11" s="18">
         <v>160</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="6"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
-      <c r="H12" s="40"/>
-      <c r="I12" s="40"/>
-      <c r="J12" s="40"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="16"/>
-      <c r="N12" s="6"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="32" t="s">
+      <c r="A13" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
-      <c r="H13" s="40"/>
-      <c r="I13" s="40"/>
-      <c r="J13" s="40"/>
-      <c r="K13" s="1"/>
-      <c r="M13" s="16"/>
-      <c r="N13" s="6"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="1"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="16"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="7"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
       <c r="K14" s="1"/>
-      <c r="M14" s="16"/>
+      <c r="M14" s="14"/>
       <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="16"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="7"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
       <c r="K15" s="1"/>
-      <c r="M15" s="16"/>
+      <c r="M15" s="14"/>
       <c r="N15" s="6"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="47">
+      <c r="A16" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="42">
         <v>0</v>
       </c>
-      <c r="C16" s="48">
+      <c r="C16" s="43">
         <v>0</v>
       </c>
       <c r="D16" s="6"/>
@@ -1702,241 +1761,241 @@
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
       <c r="K16" s="1"/>
-      <c r="M16" s="16"/>
+      <c r="M16" s="14"/>
       <c r="N16" s="6"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I17" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="J17" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="L17" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="N17" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="O17" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="J17" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="L17" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="M17" s="33" t="s">
-        <v>26</v>
-      </c>
-      <c r="N17" s="33" t="s">
-        <v>25</v>
-      </c>
-      <c r="O17" s="34" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B18" s="35">
+      <c r="B18" s="33">
         <f>$B$8</f>
         <v>50</v>
       </c>
-      <c r="C18" s="21">
-        <f>D8</f>
+      <c r="C18" s="19">
+        <f>C8</f>
         <v>50</v>
       </c>
-      <c r="D18" s="21">
+      <c r="D18" s="19">
         <f>$B$8</f>
         <v>50</v>
       </c>
-      <c r="E18" s="21">
-        <f>D8+E8</f>
+      <c r="E18" s="19">
+        <f>C8+D8</f>
         <v>130</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="19">
         <f>$B$8</f>
         <v>50</v>
       </c>
-      <c r="G18" s="21">
-        <f>E18+F8</f>
+      <c r="G18" s="19">
+        <f>E18+E8</f>
         <v>290</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="19">
         <f>$B$8</f>
         <v>50</v>
       </c>
-      <c r="I18" s="21">
-        <f>G18+G8</f>
+      <c r="I18" s="19">
+        <f>G18+F8</f>
         <v>370</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="K18" s="40"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="40"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="38"/>
+      <c r="O18" s="38"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="36">
+      <c r="A19" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="34">
         <f>B18+$B9</f>
         <v>130</v>
       </c>
-      <c r="C19" s="20">
-        <f t="shared" ref="C19:E23" si="0">D9</f>
+      <c r="C19" s="18">
+        <f>C9</f>
         <v>50</v>
       </c>
-      <c r="D19" s="20">
+      <c r="D19" s="18">
         <f>D18+$B9</f>
         <v>130</v>
       </c>
-      <c r="E19" s="20">
-        <f>D9+E9</f>
+      <c r="E19" s="18">
+        <f>C9+D9</f>
         <v>130</v>
       </c>
-      <c r="F19" s="20">
+      <c r="F19" s="18">
         <f>F18+$B9</f>
         <v>130</v>
       </c>
-      <c r="G19" s="20">
-        <f>E19+F9</f>
+      <c r="G19" s="18">
+        <f>E19+E9</f>
         <v>290</v>
       </c>
-      <c r="H19" s="20">
+      <c r="H19" s="18">
         <f>H18+$B9</f>
         <v>130</v>
       </c>
-      <c r="I19" s="20">
-        <f>G19+G9</f>
+      <c r="I19" s="18">
+        <f>G19+F9</f>
         <v>370</v>
       </c>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="40"/>
-      <c r="N19" s="40"/>
-      <c r="O19" s="40"/>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="38"/>
+      <c r="O19" s="38"/>
     </row>
     <row r="20" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B20" s="36">
+      <c r="A20" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="34">
         <f>B19+$B10</f>
         <v>210</v>
       </c>
-      <c r="C20" s="20">
-        <f t="shared" si="0"/>
+      <c r="C20" s="18">
+        <f>C10</f>
         <v>50</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D20" s="18">
         <f>D19+$B10</f>
         <v>210</v>
       </c>
-      <c r="E20" s="20">
-        <f>D10+E10</f>
+      <c r="E20" s="18">
+        <f>C10+D10</f>
         <v>370</v>
       </c>
-      <c r="F20" s="40"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="40"/>
-      <c r="I20" s="40"/>
-      <c r="J20" s="40"/>
-      <c r="K20" s="40"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="40"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="38"/>
+      <c r="N20" s="38"/>
+      <c r="O20" s="38"/>
     </row>
     <row r="21" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="36">
+      <c r="A21" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" s="34">
         <f>B20+$B11</f>
         <v>290</v>
       </c>
-      <c r="C21" s="20">
-        <f t="shared" si="0"/>
+      <c r="C21" s="18">
+        <f>C11</f>
         <v>130</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="18">
         <f>D20+$B11</f>
         <v>290</v>
       </c>
-      <c r="E21" s="20">
-        <f>D11+E11</f>
+      <c r="E21" s="18">
+        <f>C11+D11</f>
         <v>290</v>
       </c>
-      <c r="F21" s="40"/>
-      <c r="G21" s="40"/>
-      <c r="H21" s="40"/>
-      <c r="I21" s="40"/>
-      <c r="J21" s="40"/>
-      <c r="K21" s="40"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="40"/>
-      <c r="N21" s="40"/>
-      <c r="O21" s="40"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="38"/>
+      <c r="N21" s="38"/>
+      <c r="O21" s="38"/>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="38"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
+    </row>
+    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
-      <c r="I22" s="40"/>
-      <c r="J22" s="40"/>
-      <c r="K22" s="40"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="40"/>
-      <c r="N22" s="40"/>
-      <c r="O22" s="40"/>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="40"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="40"/>
-      <c r="J23" s="40"/>
-      <c r="K23" s="40"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="40"/>
-      <c r="O23" s="40"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="38"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
@@ -1965,256 +2024,246 @@
       <c r="K25" s="1"/>
     </row>
     <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="41" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="43"/>
+      <c r="A26" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="54"/>
+      <c r="E26" s="54"/>
+      <c r="F26" s="54"/>
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="46"/>
       <c r="K26" s="1"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
+      <c r="A27" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" s="21">
+        <v>4</v>
+      </c>
+      <c r="C27" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="23">
-        <v>4</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="23" t="s">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="22"/>
+      <c r="J27" s="1"/>
+    </row>
+    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="23"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G28" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="1"/>
-    </row>
-    <row r="28" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="25"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="E28" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="F28" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="G28" s="27" t="s">
-        <v>23</v>
-      </c>
-      <c r="H28" s="27" t="s">
+      <c r="H28" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="I28" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="J28" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="K28" s="1"/>
+      <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="B29" s="30">
+      <c r="B29" s="28">
+        <v>0</v>
+      </c>
+      <c r="C29" s="28">
         <v>50</v>
       </c>
-      <c r="C29" s="30">
-        <v>4</v>
-      </c>
-      <c r="D29" s="30">
+      <c r="D29" s="28">
+        <v>80</v>
+      </c>
+      <c r="E29" s="28">
+        <v>160</v>
+      </c>
+      <c r="F29" s="28">
+        <v>80</v>
+      </c>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="5"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="5"/>
+    </row>
+    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="18">
+        <v>80</v>
+      </c>
+      <c r="C30" s="18">
         <v>50</v>
       </c>
-      <c r="E29" s="30">
-        <v>80</v>
-      </c>
-      <c r="F29" s="30">
+      <c r="D30" s="18">
+        <v>80</v>
+      </c>
+      <c r="E30" s="18">
         <v>160</v>
       </c>
-      <c r="G29" s="30">
-        <v>80</v>
-      </c>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="5"/>
-    </row>
-    <row r="30" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="20">
-        <v>80</v>
-      </c>
-      <c r="C30" s="20">
-        <v>4</v>
-      </c>
-      <c r="D30" s="20">
+      <c r="F30" s="18">
+        <v>80</v>
+      </c>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+    </row>
+    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="18">
+        <v>80</v>
+      </c>
+      <c r="C31" s="18">
         <v>50</v>
       </c>
-      <c r="E30" s="20">
-        <v>80</v>
-      </c>
-      <c r="F30" s="20">
+      <c r="D31" s="18">
+        <v>80</v>
+      </c>
+      <c r="E31" s="18">
         <v>160</v>
       </c>
-      <c r="G30" s="20">
-        <v>80</v>
-      </c>
-      <c r="H30" s="40"/>
-      <c r="I30" s="40"/>
-      <c r="J30" s="40"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="6"/>
-      <c r="O30" s="6"/>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="B31" s="20">
-        <v>80</v>
-      </c>
-      <c r="C31" s="20">
-        <v>2</v>
-      </c>
-      <c r="D31" s="20">
+      <c r="F31" s="18">
+        <v>80</v>
+      </c>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="2"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="6"/>
+    </row>
+    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="18">
+        <v>80</v>
+      </c>
+      <c r="C32" s="18">
         <v>50</v>
       </c>
-      <c r="E31" s="20">
-        <v>320</v>
-      </c>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="16"/>
-      <c r="N31" s="6"/>
-    </row>
-    <row r="32" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="20">
-        <v>80</v>
-      </c>
-      <c r="C32" s="20">
-        <v>2</v>
-      </c>
-      <c r="D32" s="20">
-        <v>130</v>
-      </c>
-      <c r="E32" s="20">
+      <c r="D32" s="18">
+        <v>80</v>
+      </c>
+      <c r="E32" s="18">
         <v>160</v>
       </c>
-      <c r="F32" s="40"/>
-      <c r="G32" s="40"/>
-      <c r="H32" s="40"/>
-      <c r="I32" s="40"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="6"/>
+      <c r="F32" s="18">
+        <v>80</v>
+      </c>
+      <c r="G32" s="38"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="38"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="2"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="6"/>
     </row>
     <row r="33" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="6"/>
+      <c r="B33" s="38"/>
+      <c r="C33" s="38"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="2"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="6"/>
     </row>
     <row r="34" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="32" t="s">
+      <c r="A34" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
-      <c r="D34" s="40"/>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="1"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="6"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="38"/>
+      <c r="D34" s="38"/>
+      <c r="E34" s="38"/>
+      <c r="F34" s="38"/>
+      <c r="G34" s="38"/>
+      <c r="H34" s="38"/>
+      <c r="I34" s="38"/>
+      <c r="J34" s="1"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="6"/>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A35" s="16"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="7"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
       <c r="K35" s="1"/>
-      <c r="M35" s="16"/>
+      <c r="M35" s="14"/>
       <c r="N35" s="6"/>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="16"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="7"/>
-      <c r="C36" s="18"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
       <c r="K36" s="1"/>
-      <c r="M36" s="16"/>
+      <c r="M36" s="14"/>
       <c r="N36" s="6"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="46" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" s="47">
-        <f>D2</f>
-        <v>8050</v>
-      </c>
-      <c r="C37" s="48">
+      <c r="A37" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="42">
+        <f>$D$2/2-MAX(B39:B44)/2</f>
+        <v>3905</v>
+      </c>
+      <c r="C37" s="43">
         <v>0</v>
       </c>
       <c r="D37" s="6"/>
@@ -2225,256 +2274,937 @@
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
       <c r="K37" s="1"/>
-      <c r="M37" s="16"/>
+      <c r="M37" s="14"/>
       <c r="N37" s="6"/>
     </row>
     <row r="38" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="40" t="s">
+        <v>26</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="F38" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G38" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="I38" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="J38" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="K38" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="L38" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="M38" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="N38" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="O38" s="32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B38" s="45" t="s">
+      <c r="B39" s="33">
+        <f>$B29</f>
+        <v>0</v>
+      </c>
+      <c r="C39" s="19">
+        <f>C29</f>
+        <v>50</v>
+      </c>
+      <c r="D39" s="33">
+        <f>$B29</f>
+        <v>0</v>
+      </c>
+      <c r="E39" s="19">
+        <f>C29+D29</f>
+        <v>130</v>
+      </c>
+      <c r="F39" s="33">
+        <f>$B29</f>
+        <v>0</v>
+      </c>
+      <c r="G39" s="19">
+        <f>E39+E29</f>
+        <v>290</v>
+      </c>
+      <c r="H39" s="33">
+        <f>$B29</f>
+        <v>0</v>
+      </c>
+      <c r="I39" s="19">
+        <f>G39+F29</f>
+        <v>370</v>
+      </c>
+      <c r="J39" s="38"/>
+      <c r="K39" s="38"/>
+      <c r="L39" s="38"/>
+      <c r="M39" s="38"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="38"/>
+    </row>
+    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B40" s="34">
+        <f>B39+$B30</f>
+        <v>80</v>
+      </c>
+      <c r="C40" s="19">
+        <f t="shared" ref="C40:C43" si="0">C30</f>
+        <v>50</v>
+      </c>
+      <c r="D40" s="34">
+        <f>D39+$B30</f>
+        <v>80</v>
+      </c>
+      <c r="E40" s="18">
+        <f>C30+D30</f>
+        <v>130</v>
+      </c>
+      <c r="F40" s="34">
+        <f>F39+$B30</f>
+        <v>80</v>
+      </c>
+      <c r="G40" s="19">
+        <f t="shared" ref="G40:G43" si="1">E40+E30</f>
+        <v>290</v>
+      </c>
+      <c r="H40" s="34">
+        <f>H39+$B30</f>
+        <v>80</v>
+      </c>
+      <c r="I40" s="19">
+        <f t="shared" ref="I40:I43" si="2">G40+F30</f>
+        <v>370</v>
+      </c>
+      <c r="J40" s="38"/>
+      <c r="K40" s="38"/>
+      <c r="L40" s="38"/>
+      <c r="M40" s="38"/>
+      <c r="N40" s="38"/>
+      <c r="O40" s="38"/>
+    </row>
+    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B41" s="34">
+        <f>B40+$B31</f>
+        <v>160</v>
+      </c>
+      <c r="C41" s="19">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D41" s="34">
+        <f>D40+$B31</f>
+        <v>160</v>
+      </c>
+      <c r="E41" s="18">
+        <f>C31+D31</f>
+        <v>130</v>
+      </c>
+      <c r="F41" s="34">
+        <f>F40+$B31</f>
+        <v>160</v>
+      </c>
+      <c r="G41" s="19">
+        <f t="shared" si="1"/>
+        <v>290</v>
+      </c>
+      <c r="H41" s="34">
+        <f>H40+$B31</f>
+        <v>160</v>
+      </c>
+      <c r="I41" s="19">
+        <f t="shared" si="2"/>
+        <v>370</v>
+      </c>
+      <c r="J41" s="38"/>
+      <c r="K41" s="38"/>
+      <c r="L41" s="38"/>
+      <c r="M41" s="38"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="38"/>
+    </row>
+    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="34">
+        <f>B41+$B32</f>
+        <v>240</v>
+      </c>
+      <c r="C42" s="19">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D42" s="34">
+        <f>D41+$B32</f>
+        <v>240</v>
+      </c>
+      <c r="E42" s="18">
+        <f>C32+D32</f>
+        <v>130</v>
+      </c>
+      <c r="F42" s="34">
+        <f>F41+$B32</f>
+        <v>240</v>
+      </c>
+      <c r="G42" s="19">
+        <f t="shared" si="1"/>
+        <v>290</v>
+      </c>
+      <c r="H42" s="34">
+        <f>H41+$B32</f>
+        <v>240</v>
+      </c>
+      <c r="I42" s="19">
+        <f t="shared" si="2"/>
+        <v>370</v>
+      </c>
+      <c r="J42" s="38"/>
+      <c r="K42" s="38"/>
+      <c r="L42" s="38"/>
+      <c r="M42" s="38"/>
+      <c r="N42" s="38"/>
+      <c r="O42" s="38"/>
+    </row>
+    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B43" s="38"/>
+      <c r="C43" s="38"/>
+      <c r="D43" s="38"/>
+      <c r="E43" s="38"/>
+      <c r="F43" s="38"/>
+      <c r="G43" s="38"/>
+      <c r="H43" s="38"/>
+      <c r="I43" s="38"/>
+      <c r="J43" s="38"/>
+      <c r="K43" s="38"/>
+      <c r="L43" s="38"/>
+      <c r="M43" s="38"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+    </row>
+    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="38"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="38"/>
+      <c r="E44" s="38"/>
+      <c r="F44" s="38"/>
+      <c r="G44" s="38"/>
+      <c r="H44" s="38"/>
+      <c r="I44" s="38"/>
+      <c r="J44" s="38"/>
+      <c r="K44" s="38"/>
+      <c r="L44" s="38"/>
+      <c r="M44" s="38"/>
+      <c r="N44" s="38"/>
+      <c r="O44" s="38"/>
+    </row>
+    <row r="46" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="54"/>
+      <c r="C47" s="54"/>
+      <c r="D47" s="54"/>
+      <c r="E47" s="54"/>
+      <c r="F47" s="54"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="54"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="46"/>
+      <c r="K47" s="1"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" s="21">
+        <v>4</v>
+      </c>
+      <c r="C48" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="22"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="23"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="F49" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G49" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="H49" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I49" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" s="44">
+        <v>50</v>
+      </c>
+      <c r="C50" s="44">
+        <v>63</v>
+      </c>
+      <c r="D50" s="44">
+        <v>80</v>
+      </c>
+      <c r="E50" s="44">
+        <v>80</v>
+      </c>
+      <c r="F50" s="44">
+        <v>80</v>
+      </c>
+      <c r="G50" s="44">
+        <v>80</v>
+      </c>
+      <c r="H50" s="44">
+        <v>80</v>
+      </c>
+      <c r="I50" s="38"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="5"/>
+    </row>
+    <row r="51" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51" s="45">
+        <v>80</v>
+      </c>
+      <c r="C51" s="45">
+        <v>63</v>
+      </c>
+      <c r="D51" s="45">
+        <v>80</v>
+      </c>
+      <c r="E51" s="45">
+        <v>80</v>
+      </c>
+      <c r="F51" s="45">
+        <v>80</v>
+      </c>
+      <c r="G51" s="45">
+        <v>80</v>
+      </c>
+      <c r="H51" s="45">
+        <v>80</v>
+      </c>
+      <c r="I51" s="38"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+    </row>
+    <row r="52" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B52" s="45">
+        <v>80</v>
+      </c>
+      <c r="C52" s="45">
+        <v>63</v>
+      </c>
+      <c r="D52" s="45">
+        <v>80</v>
+      </c>
+      <c r="E52" s="44">
+        <v>80</v>
+      </c>
+      <c r="F52" s="44">
+        <v>80</v>
+      </c>
+      <c r="G52" s="44">
+        <v>80</v>
+      </c>
+      <c r="H52" s="44">
+        <v>80</v>
+      </c>
+      <c r="I52" s="38"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="2"/>
+      <c r="L52" s="14"/>
+      <c r="M52" s="6"/>
+    </row>
+    <row r="53" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B53" s="38"/>
+      <c r="C53" s="38"/>
+      <c r="D53" s="38"/>
+      <c r="E53" s="38"/>
+      <c r="F53" s="38"/>
+      <c r="G53" s="38"/>
+      <c r="H53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="6"/>
+    </row>
+    <row r="54" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B54" s="38"/>
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+      <c r="I54" s="38"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="2"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="6"/>
+    </row>
+    <row r="55" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B55" s="38"/>
+      <c r="C55" s="38"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
+      <c r="I55" s="38"/>
+      <c r="J55" s="1"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="6"/>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="14"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="16"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
+      <c r="F56" s="17"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+      <c r="J56" s="17"/>
+      <c r="K56" s="1"/>
+      <c r="M56" s="14"/>
+      <c r="N56" s="6"/>
+    </row>
+    <row r="57" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="14"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="16"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
+      <c r="F57" s="17"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+      <c r="J57" s="17"/>
+      <c r="K57" s="1"/>
+      <c r="M57" s="14"/>
+      <c r="N57" s="6"/>
+    </row>
+    <row r="58" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B58" s="42">
+        <v>0</v>
+      </c>
+      <c r="C58" s="43">
+        <v>0</v>
+      </c>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+      <c r="K58" s="1"/>
+      <c r="M58" s="14"/>
+      <c r="N58" s="6"/>
+    </row>
+    <row r="59" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C38" s="45" t="s">
+      <c r="C59" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="D38" s="33" t="s">
+      <c r="D59" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="33" t="s">
+      <c r="E59" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="33" t="s">
+      <c r="F59" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G38" s="33" t="s">
+      <c r="G59" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H38" s="33" t="s">
+      <c r="H59" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="I38" s="33" t="s">
+      <c r="I59" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="J38" s="33" t="s">
+      <c r="J59" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="K38" s="33" t="s">
+      <c r="K59" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="L38" s="33" t="s">
+      <c r="L59" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="M38" s="33" t="s">
+      <c r="M59" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="N38" s="33" t="s">
+      <c r="N59" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="O38" s="34" t="s">
+      <c r="O59" s="32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="37" t="s">
+    <row r="60" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B60" s="33">
+        <f>$B50</f>
+        <v>50</v>
+      </c>
+      <c r="C60" s="19">
+        <f>C50</f>
+        <v>63</v>
+      </c>
+      <c r="D60" s="33">
+        <f>$B50</f>
+        <v>50</v>
+      </c>
+      <c r="E60" s="19">
+        <f>C60+D50</f>
+        <v>143</v>
+      </c>
+      <c r="F60" s="33">
+        <f>$B50</f>
+        <v>50</v>
+      </c>
+      <c r="G60" s="19">
+        <f>E60+E50</f>
+        <v>223</v>
+      </c>
+      <c r="H60" s="33">
+        <f>$B50</f>
+        <v>50</v>
+      </c>
+      <c r="I60" s="19">
+        <f>G60+F50</f>
+        <v>303</v>
+      </c>
+      <c r="J60" s="33">
+        <f>$B50</f>
+        <v>50</v>
+      </c>
+      <c r="K60" s="19">
+        <f>I60+G50</f>
+        <v>383</v>
+      </c>
+      <c r="L60" s="33">
+        <f>$B50</f>
+        <v>50</v>
+      </c>
+      <c r="M60" s="19">
+        <f>K60+H50</f>
+        <v>463</v>
+      </c>
+      <c r="N60" s="38"/>
+      <c r="O60" s="38"/>
+    </row>
+    <row r="61" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="35">
-        <f>$B$29</f>
+      <c r="B61" s="34">
+        <f>B60+$B51</f>
+        <v>130</v>
+      </c>
+      <c r="C61" s="18">
+        <f t="shared" ref="C61:E61" si="3">C51</f>
+        <v>63</v>
+      </c>
+      <c r="D61" s="34">
+        <f>D60+$B51</f>
+        <v>130</v>
+      </c>
+      <c r="E61" s="19">
+        <f t="shared" ref="E61:E62" si="4">C61+D51</f>
+        <v>143</v>
+      </c>
+      <c r="F61" s="34">
+        <f>F60+$B51</f>
+        <v>130</v>
+      </c>
+      <c r="G61" s="19">
+        <f t="shared" ref="G61:M62" si="5">E61+E51</f>
+        <v>223</v>
+      </c>
+      <c r="H61" s="34">
+        <f>H60+$B51</f>
+        <v>130</v>
+      </c>
+      <c r="I61" s="19">
+        <f t="shared" ref="I61:I62" si="6">G61+F51</f>
+        <v>303</v>
+      </c>
+      <c r="J61" s="34">
+        <f>J60+$B51</f>
+        <v>130</v>
+      </c>
+      <c r="K61" s="19">
+        <f t="shared" ref="K61:K62" si="7">I61+G51</f>
+        <v>383</v>
+      </c>
+      <c r="L61" s="34">
+        <f>L60+$B51</f>
+        <v>130</v>
+      </c>
+      <c r="M61" s="19">
+        <f t="shared" ref="M61:M62" si="8">K61+H51</f>
+        <v>463</v>
+      </c>
+      <c r="N61" s="38"/>
+      <c r="O61" s="38"/>
+    </row>
+    <row r="62" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="B62" s="34">
+        <f>B61+$B52</f>
+        <v>210</v>
+      </c>
+      <c r="C62" s="18">
+        <f t="shared" ref="C62:E62" si="9">C52</f>
+        <v>63</v>
+      </c>
+      <c r="D62" s="34">
+        <f>D61+$B52</f>
+        <v>210</v>
+      </c>
+      <c r="E62" s="19">
+        <f t="shared" si="4"/>
+        <v>143</v>
+      </c>
+      <c r="F62" s="34">
+        <f>F61+$B52</f>
+        <v>210</v>
+      </c>
+      <c r="G62" s="19">
+        <f t="shared" si="5"/>
+        <v>223</v>
+      </c>
+      <c r="H62" s="34">
+        <f>H61+$B52</f>
+        <v>210</v>
+      </c>
+      <c r="I62" s="19">
+        <f t="shared" si="6"/>
+        <v>303</v>
+      </c>
+      <c r="J62" s="34">
+        <f>J61+$B52</f>
+        <v>210</v>
+      </c>
+      <c r="K62" s="19">
+        <f t="shared" si="7"/>
+        <v>383</v>
+      </c>
+      <c r="L62" s="34">
+        <f>L61+$B52</f>
+        <v>210</v>
+      </c>
+      <c r="M62" s="19">
+        <f t="shared" si="8"/>
+        <v>463</v>
+      </c>
+      <c r="N62" s="38"/>
+      <c r="O62" s="38"/>
+    </row>
+    <row r="63" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B63" s="38"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="38"/>
+      <c r="E63" s="38"/>
+      <c r="F63" s="38"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="38"/>
+      <c r="I63" s="38"/>
+      <c r="J63" s="38"/>
+      <c r="K63" s="38"/>
+      <c r="L63" s="38"/>
+      <c r="M63" s="38"/>
+      <c r="N63" s="38"/>
+      <c r="O63" s="38"/>
+    </row>
+    <row r="64" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B64" s="38"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="38"/>
+      <c r="E64" s="38"/>
+      <c r="F64" s="38"/>
+      <c r="G64" s="38"/>
+      <c r="H64" s="38"/>
+      <c r="I64" s="38"/>
+      <c r="J64" s="38"/>
+      <c r="K64" s="38"/>
+      <c r="L64" s="38"/>
+      <c r="M64" s="38"/>
+      <c r="N64" s="38"/>
+      <c r="O64" s="38"/>
+    </row>
+    <row r="65" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B65" s="38"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="38"/>
+      <c r="E65" s="38"/>
+      <c r="F65" s="38"/>
+      <c r="G65" s="38"/>
+      <c r="H65" s="38"/>
+      <c r="I65" s="38"/>
+      <c r="J65" s="38"/>
+      <c r="K65" s="38"/>
+      <c r="L65" s="38"/>
+      <c r="M65" s="38"/>
+      <c r="N65" s="38"/>
+      <c r="O65" s="38"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="48"/>
+      <c r="B69" s="2">
+        <f>B18</f>
         <v>50</v>
       </c>
-      <c r="C39" s="21">
-        <f>D29</f>
-        <v>50</v>
-      </c>
-      <c r="D39" s="21">
-        <f>$B$8</f>
-        <v>50</v>
-      </c>
-      <c r="E39" s="21">
-        <f>D29+E29</f>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="48"/>
+      <c r="B70" s="2">
+        <f t="shared" ref="B70:B74" si="10">B19</f>
         <v>130</v>
       </c>
-      <c r="F39" s="21">
-        <f>$B$8</f>
-        <v>50</v>
-      </c>
-      <c r="G39" s="21">
-        <f>E39+F29</f>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="48"/>
+      <c r="B71" s="2">
+        <f t="shared" si="10"/>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="48"/>
+      <c r="B72" s="2">
+        <f t="shared" si="10"/>
         <v>290</v>
       </c>
-      <c r="H39" s="21">
-        <f>$B$8</f>
-        <v>50</v>
-      </c>
-      <c r="I39" s="21">
-        <f>G39+G29</f>
-        <v>370</v>
-      </c>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="40"/>
-      <c r="N39" s="40"/>
-      <c r="O39" s="40"/>
-    </row>
-    <row r="40" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="36">
-        <f>B39+$B30</f>
-        <v>130</v>
-      </c>
-      <c r="C40" s="20">
-        <f t="shared" ref="C40:E40" si="1">D30</f>
-        <v>50</v>
-      </c>
-      <c r="D40" s="20">
-        <f>D39+$B30</f>
-        <v>130</v>
-      </c>
-      <c r="E40" s="20">
-        <f>D30+E30</f>
-        <v>130</v>
-      </c>
-      <c r="F40" s="20">
-        <f>F39+$B30</f>
-        <v>130</v>
-      </c>
-      <c r="G40" s="20">
-        <f>E40+F30</f>
-        <v>290</v>
-      </c>
-      <c r="H40" s="20">
-        <f>H39+$B30</f>
-        <v>130</v>
-      </c>
-      <c r="I40" s="20">
-        <f>G40+G30</f>
-        <v>370</v>
-      </c>
-      <c r="J40" s="40"/>
-      <c r="K40" s="40"/>
-      <c r="L40" s="40"/>
-      <c r="M40" s="40"/>
-      <c r="N40" s="40"/>
-      <c r="O40" s="40"/>
-    </row>
-    <row r="41" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="B41" s="36">
-        <f>B40+$B31</f>
-        <v>210</v>
-      </c>
-      <c r="C41" s="20">
-        <f t="shared" ref="C41:E41" si="2">D31</f>
-        <v>50</v>
-      </c>
-      <c r="D41" s="20">
-        <f>D40+$B31</f>
-        <v>210</v>
-      </c>
-      <c r="E41" s="20">
-        <f>D31+E31</f>
-        <v>370</v>
-      </c>
-      <c r="F41" s="40"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="40"/>
-      <c r="I41" s="40"/>
-      <c r="J41" s="40"/>
-      <c r="K41" s="40"/>
-      <c r="L41" s="40"/>
-      <c r="M41" s="40"/>
-      <c r="N41" s="40"/>
-      <c r="O41" s="40"/>
-    </row>
-    <row r="42" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B42" s="36">
-        <f>B41+$B32</f>
-        <v>290</v>
-      </c>
-      <c r="C42" s="20">
-        <f t="shared" ref="C42:E42" si="3">D32</f>
-        <v>130</v>
-      </c>
-      <c r="D42" s="20">
-        <f>D41+$B32</f>
-        <v>290</v>
-      </c>
-      <c r="E42" s="20">
-        <f>D32+E32</f>
-        <v>290</v>
-      </c>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
-      <c r="I42" s="40"/>
-      <c r="J42" s="40"/>
-      <c r="K42" s="40"/>
-      <c r="L42" s="40"/>
-      <c r="M42" s="40"/>
-      <c r="N42" s="40"/>
-      <c r="O42" s="40"/>
-    </row>
-    <row r="43" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="38" t="s">
-        <v>37</v>
-      </c>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
-      <c r="F43" s="40"/>
-      <c r="G43" s="40"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
-      <c r="K43" s="40"/>
-      <c r="L43" s="40"/>
-      <c r="M43" s="40"/>
-      <c r="N43" s="40"/>
-      <c r="O43" s="40"/>
-    </row>
-    <row r="44" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
-      <c r="F44" s="40"/>
-      <c r="G44" s="40"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
-      <c r="K44" s="40"/>
-      <c r="L44" s="40"/>
-      <c r="M44" s="40"/>
-      <c r="N44" s="40"/>
-      <c r="O44" s="40"/>
+    </row>
+    <row r="73" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="48"/>
+      <c r="B73" s="38"/>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A74" s="48"/>
+      <c r="B74" s="38"/>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B75" s="2">
+        <f>$B$37+B39</f>
+        <v>3905</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A76" s="48"/>
+      <c r="B76" s="2">
+        <f t="shared" ref="B76:B80" si="11">$B$37+B40</f>
+        <v>3985</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A77" s="48"/>
+      <c r="B77" s="2">
+        <f t="shared" si="11"/>
+        <v>4065</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="48"/>
+      <c r="B78" s="2">
+        <f t="shared" si="11"/>
+        <v>4145</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="48"/>
+      <c r="B79" s="38"/>
+    </row>
+    <row r="80" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="48"/>
+      <c r="B80" s="38"/>
+    </row>
+    <row r="81" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B81" s="38"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="48"/>
+      <c r="B82" s="38"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="48"/>
+      <c r="B83" s="2">
+        <f>$D$2-B72</f>
+        <v>7760</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="48"/>
+      <c r="B84" s="2">
+        <f>$D$2-B71</f>
+        <v>7840</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="48"/>
+      <c r="B85" s="2">
+        <f>$D$2-B70</f>
+        <v>7920</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="48"/>
+      <c r="B86" s="2">
+        <f>$D$2-B69</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="48"/>
+      <c r="B87" s="2">
+        <f>$D$2</f>
+        <v>8050</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A26:J26"/>
+  <mergeCells count="15">
+    <mergeCell ref="A75:A80"/>
+    <mergeCell ref="A68:A74"/>
+    <mergeCell ref="A81:A87"/>
+    <mergeCell ref="A48:A49"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="C48:I48"/>
+    <mergeCell ref="A5:I5"/>
+    <mergeCell ref="A26:I26"/>
+    <mergeCell ref="A47:I47"/>
     <mergeCell ref="A27:A28"/>
     <mergeCell ref="B27:B28"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:J27"/>
+    <mergeCell ref="C27:I27"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A5:J5"/>
+    <mergeCell ref="C6:I6"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A4">
       <formula1>elements</formula1>
     </dataValidation>

</xml_diff>